<commit_message>
fix(datamodel): Fix make thirteen 13 in employees
</commit_message>
<xml_diff>
--- a/very_advanced_data_example.xlsx
+++ b/very_advanced_data_example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="921" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14260" tabRatio="921" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="6" r:id="rId1"/>
@@ -3715,8 +3715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4143,7 +4143,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>536</v>
@@ -4195,7 +4195,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>556</v>
@@ -6599,7 +6599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
@@ -8921,7 +8921,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>